<commit_message>
Feature importance for taken formula
</commit_message>
<xml_diff>
--- a/lastseason/lastseasoniplbatting.xlsx
+++ b/lastseason/lastseasoniplbatting.xlsx
@@ -40,10 +40,10 @@
     <t>SR</t>
   </si>
   <si>
-    <t>100's</t>
-  </si>
-  <si>
-    <t>50's</t>
+    <t>100s</t>
+  </si>
+  <si>
+    <t>50s</t>
   </si>
   <si>
     <t>4s</t>
@@ -966,9 +966,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1048,7 +1048,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1075,10 +1075,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1325,9 +1325,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1605,7 +1605,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1632,10 +1632,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>